<commit_message>
adicionei o começo do dash ka
</commit_message>
<xml_diff>
--- a/4.Site/Index/DASHBOARD-EVA-20.04.xlsx
+++ b/4.Site/Index/DASHBOARD-EVA-20.04.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus Vinícius\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milene Oliveira\Documents\sprint\eva\4.Site\Index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE4E637-4DD2-4717-A72E-0C315730F545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC98830-FBF6-4D67-8800-E693A4DA27FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64C60D2E-F752-464D-A341-317F01FE6D45}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -6257,8 +6259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28FBD0A-7D15-4976-B634-2946DCC81DDC}">
   <dimension ref="B1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52:I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6470,7 +6472,7 @@
     </row>
     <row r="52" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I52" s="69">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="53" spans="9:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6494,8 +6496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5F3198-1182-4A20-89AB-AA99E7D67846}">
   <dimension ref="A3:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>